<commit_message>
Updated font sizes across the whole sheet... adding css variables for each.
</commit_message>
<xml_diff>
--- a/css_variable_font_sizes.xlsx
+++ b/css_variable_font_sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\css_modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\code\css_modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3E0555-E30A-4C78-88AA-2E5AD1B025C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE73C59-9B3D-436D-8D46-4FA3B389656E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F820B3DE-D05A-4853-9D82-A8DA71430E49}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F820B3DE-D05A-4853-9D82-A8DA71430E49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Heading</t>
   </si>
@@ -94,6 +94,30 @@
   </si>
   <si>
     <t>text4</t>
+  </si>
+  <si>
+    <t>h6-a</t>
+  </si>
+  <si>
+    <t>h1-a</t>
+  </si>
+  <si>
+    <t>h2-a</t>
+  </si>
+  <si>
+    <t>h3-a</t>
+  </si>
+  <si>
+    <t>h4-a</t>
+  </si>
+  <si>
+    <t>h5-a</t>
+  </si>
+  <si>
+    <t>--step--1</t>
+  </si>
+  <si>
+    <t>--step--2</t>
   </si>
 </sst>
 </file>
@@ -185,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +251,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -543,22 +570,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5A6C22-BA9E-45E6-91AE-D25F7D23ED5A}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="2"/>
-    <col min="2" max="17" width="8.75" style="3"/>
-    <col min="18" max="18" width="9.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.75" style="1"/>
+    <col min="1" max="1" width="8.69921875" style="2"/>
+    <col min="2" max="17" width="8.69921875" style="3"/>
+    <col min="18" max="18" width="9.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.09765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -617,7 +645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -688,7 +716,7 @@
         <v>font-size: clamp(2rem, 1.5vw + 1.25rem, 3rem);</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -756,11 +784,11 @@
         <v>2.4000000000000004</v>
       </c>
       <c r="S3" s="12" t="str">
-        <f t="shared" ref="S3:S12" si="6">"font-size: clamp("&amp;D3&amp;"rem, "&amp;B3&amp;"vw + "&amp;C3&amp;"rem, "&amp;J3&amp;"rem);"</f>
+        <f t="shared" ref="S3:S11" si="6">"font-size: clamp("&amp;D3&amp;"rem, "&amp;B3&amp;"vw + "&amp;C3&amp;"rem, "&amp;J3&amp;"rem);"</f>
         <v>font-size: clamp(1.6rem, 1.2vw + 1rem, 2.4rem);</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -832,7 +860,7 @@
         <v>font-size: clamp(1.4rem, 1vw + 0.9rem, 2.1rem);</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -904,7 +932,7 @@
         <v>font-size: clamp(1.2rem, 0.85vw + 0.8rem, 1.8rem);</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -976,7 +1004,7 @@
         <v>font-size: clamp(1.1rem, 0.7vw + 0.7rem, 1.5rem);</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1048,7 +1076,7 @@
         <v>font-size: clamp(1rem, 0.55vw + 0.55rem, 1.2rem);</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1114,7 +1142,7 @@
         <v>font-size: clamp(0.8rem, 0.55vw + 0.5rem, 1.1rem);</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1180,7 +1208,7 @@
         <v>font-size: clamp(1.35rem, 1.75vw + 1rem, 3rem);</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1274,7 @@
         <v>font-size: clamp(0.9rem, 0.55vw + 0.55rem, 1.1rem);</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1312,7 +1340,7 @@
         <v>font-size: clamp(0.8rem, 0.55vw + 0.5rem, 1rem);</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -1326,23 +1354,23 @@
         <v>0.9</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" ref="E12" si="29">IF(($E$1/100*B12/16)+C12&lt;D12,D12,IF(($E$1/100*B12/16)+C12&gt;J12,J12,($E$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="E12:E20" si="29">IF(($E$1/100*B12/16)+C12&lt;D12,D12,IF(($E$1/100*B12/16)+C12&gt;J12,J12,($E$1/100*B12/16)+C12))</f>
         <v>0.9</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" ref="F12" si="30">IF(($F$1/100*B12/16)+C12&lt;D12,D12,IF(($F$1/100*B12/16)+C12&gt;J12,J12,($F$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="F12:F20" si="30">IF(($F$1/100*B12/16)+C12&lt;D12,D12,IF(($F$1/100*B12/16)+C12&gt;J12,J12,($F$1/100*B12/16)+C12))</f>
         <v>0.9</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" ref="G12" si="31">IF(($G$1/100*B12/16)+C12&lt;D12,D12,IF(($G$1/100*B12/16)+C12&gt;J12,J12,($G$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="G12:G20" si="31">IF(($G$1/100*B12/16)+C12&lt;D12,D12,IF(($G$1/100*B12/16)+C12&gt;J12,J12,($G$1/100*B12/16)+C12))</f>
         <v>0.95199999999999996</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" ref="H12" si="32">IF(($H$1/100*B12/16)+C12&lt;D12,D12,IF(($H$1/100*B12/16)+C12&gt;J12,J12,($H$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="H12:H19" si="32">IF(($H$1/100*B12/16)+C12&lt;D12,D12,IF(($H$1/100*B12/16)+C12&gt;J12,J12,($H$1/100*B12/16)+C12))</f>
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" ref="I12" si="33">IF(($I$1/100*B12/16)+C12&lt;D12,D12,IF(($I$1/100*B12/16)+C12&gt;J12,J12,($I$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="I12:I19" si="33">IF(($I$1/100*B12/16)+C12&lt;D12,D12,IF(($I$1/100*B12/16)+C12&gt;J12,J12,($I$1/100*B12/16)+C12))</f>
         <v>1</v>
       </c>
       <c r="J12" s="9">
@@ -1352,23 +1380,23 @@
         <v>1</v>
       </c>
       <c r="L12" s="7">
-        <f t="shared" ref="L12" si="34">E12*16</f>
+        <f t="shared" ref="L12:L18" si="34">E12*16</f>
         <v>14.4</v>
       </c>
       <c r="M12" s="7">
-        <f t="shared" ref="M12" si="35">F12*16</f>
+        <f t="shared" ref="M12:M18" si="35">F12*16</f>
         <v>14.4</v>
       </c>
       <c r="N12" s="7">
-        <f t="shared" ref="N12" si="36">G12*16</f>
+        <f t="shared" ref="N12:N18" si="36">G12*16</f>
         <v>15.231999999999999</v>
       </c>
       <c r="O12" s="7">
-        <f t="shared" ref="O12" si="37">H12*16</f>
+        <f t="shared" ref="O12:O18" si="37">H12*16</f>
         <v>16</v>
       </c>
       <c r="P12" s="7">
-        <f t="shared" ref="P12" si="38">I12*16</f>
+        <f t="shared" ref="P12:P18" si="38">I12*16</f>
         <v>16</v>
       </c>
       <c r="Q12" s="14"/>
@@ -1378,89 +1406,554 @@
         <v>font-size: clamp(0.9rem, 0.55vw + 0.6rem, 1rem);</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
+    <row r="13" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" ref="E13:E17" si="39">IF(($E$1/100*B13/16)+C13&lt;D13,D13,IF(($E$1/100*B13/16)+C13&gt;J13,J13,($E$1/100*B13/16)+C13))</f>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" ref="F13:F17" si="40">IF(($F$1/100*B13/16)+C13&lt;D13,D13,IF(($F$1/100*B13/16)+C13&gt;J13,J13,($F$1/100*B13/16)+C13))</f>
+        <v>2.5839999999999996</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" ref="G13:G17" si="41">IF(($G$1/100*B13/16)+C13&lt;D13,D13,IF(($G$1/100*B13/16)+C13&gt;J13,J13,($G$1/100*B13/16)+C13))</f>
+        <v>2.6719999999999997</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" ref="H13:H17" si="42">IF(($H$1/100*B13/16)+C13&lt;D13,D13,IF(($H$1/100*B13/16)+C13&gt;J13,J13,($H$1/100*B13/16)+C13))</f>
+        <v>2.7895624999999997</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" ref="I13:I17" si="43">IF(($I$1/100*B13/16)+C13&lt;D13,D13,IF(($I$1/100*B13/16)+C13&gt;J13,J13,($I$1/100*B13/16)+C13))</f>
+        <v>2.98</v>
+      </c>
+      <c r="J13" s="9">
+        <v>2.99</v>
+      </c>
+      <c r="K13" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" ref="L13:L20" si="44">E13*16</f>
+        <v>39.840000000000003</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" ref="M13:M20" si="45">F13*16</f>
+        <v>41.343999999999994</v>
+      </c>
+      <c r="N13" s="7">
+        <f t="shared" ref="N13:N20" si="46">G13*16</f>
+        <v>42.751999999999995</v>
+      </c>
+      <c r="O13" s="7">
+        <f t="shared" ref="O13:O20" si="47">H13*16</f>
+        <v>44.632999999999996</v>
+      </c>
+      <c r="P13" s="7">
+        <f t="shared" ref="P13:P20" si="48">I13*16</f>
+        <v>47.68</v>
+      </c>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
-      <c r="S13" s="12"/>
-    </row>
-    <row r="14" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
+      <c r="S13" s="12" t="str">
+        <f t="shared" ref="S13:S20" si="49">"font-size: clamp("&amp;D13&amp;"rem, "&amp;B13&amp;"vw + "&amp;C13&amp;"rem, "&amp;J13&amp;"rem);"</f>
+        <v>font-size: clamp(2.49rem, 0.55vw + 2.32rem, 2.99rem);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.46</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1.94</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="39"/>
+        <v>2.0779999999999998</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="40"/>
+        <v>2.1608000000000001</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="41"/>
+        <v>2.2343999999999999</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="42"/>
+        <v>2.3327249999999999</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="43"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J14" s="9">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="K14" s="8">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="44"/>
+        <v>33.247999999999998</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="45"/>
+        <v>34.572800000000001</v>
+      </c>
+      <c r="N14" s="7">
+        <f t="shared" si="46"/>
+        <v>35.750399999999999</v>
+      </c>
+      <c r="O14" s="7">
+        <f t="shared" si="47"/>
+        <v>37.323599999999999</v>
+      </c>
+      <c r="P14" s="7">
+        <f t="shared" si="48"/>
+        <v>39.840000000000003</v>
+      </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
-      <c r="S14" s="12"/>
-    </row>
-    <row r="15" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="S14" s="12" t="str">
+        <f t="shared" si="49"/>
+        <v>font-size: clamp(2.07rem, 0.46vw + 1.94rem, 2.49rem);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.61</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1.73</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="39"/>
+        <v>1.73</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="40"/>
+        <v>1.7924000000000002</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="41"/>
+        <v>1.8532000000000002</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="42"/>
+        <v>1.9344250000000001</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="43"/>
+        <v>2.0659999999999998</v>
+      </c>
+      <c r="J15" s="9">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1.75</v>
+      </c>
+      <c r="L15" s="7">
+        <f t="shared" si="44"/>
+        <v>27.68</v>
+      </c>
+      <c r="M15" s="7">
+        <f t="shared" si="45"/>
+        <v>28.678400000000003</v>
+      </c>
+      <c r="N15" s="7">
+        <f t="shared" si="46"/>
+        <v>29.651200000000003</v>
+      </c>
+      <c r="O15" s="7">
+        <f t="shared" si="47"/>
+        <v>30.950800000000001</v>
+      </c>
+      <c r="P15" s="7">
+        <f t="shared" si="48"/>
+        <v>33.055999999999997</v>
+      </c>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
-      <c r="S15" s="12"/>
-    </row>
-    <row r="16" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="S15" s="12" t="str">
+        <f t="shared" si="49"/>
+        <v>font-size: clamp(1.73rem, 0.38vw + 1.61rem, 2.07rem);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.32</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1.34</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1.44</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="39"/>
+        <v>1.44</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="40"/>
+        <v>1.4936</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="41"/>
+        <v>1.5448000000000002</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="42"/>
+        <v>1.6132</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="43"/>
+        <v>1.7240000000000002</v>
+      </c>
+      <c r="J16" s="9">
+        <v>1.73</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="L16" s="7">
+        <f t="shared" si="44"/>
+        <v>23.04</v>
+      </c>
+      <c r="M16" s="7">
+        <f t="shared" si="45"/>
+        <v>23.897600000000001</v>
+      </c>
+      <c r="N16" s="7">
+        <f t="shared" si="46"/>
+        <v>24.716800000000003</v>
+      </c>
+      <c r="O16" s="7">
+        <f t="shared" si="47"/>
+        <v>25.811199999999999</v>
+      </c>
+      <c r="P16" s="7">
+        <f t="shared" si="48"/>
+        <v>27.584000000000003</v>
+      </c>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
-      <c r="S16" s="12"/>
+      <c r="S16" s="12" t="str">
+        <f t="shared" si="49"/>
+        <v>font-size: clamp(1.44rem, 0.32vw + 1.34rem, 1.73rem);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="39"/>
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="40"/>
+        <v>1.2496</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="41"/>
+        <v>1.2928000000000002</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="42"/>
+        <v>1.3505125000000002</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="43"/>
+        <v>1.44</v>
+      </c>
+      <c r="J17" s="9">
+        <v>1.44</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" si="44"/>
+        <v>19.216000000000001</v>
+      </c>
+      <c r="M17" s="7">
+        <f t="shared" si="45"/>
+        <v>19.993600000000001</v>
+      </c>
+      <c r="N17" s="7">
+        <f t="shared" si="46"/>
+        <v>20.684800000000003</v>
+      </c>
+      <c r="O17" s="7">
+        <f t="shared" si="47"/>
+        <v>21.608200000000004</v>
+      </c>
+      <c r="P17" s="7">
+        <f t="shared" si="48"/>
+        <v>23.04</v>
+      </c>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="12" t="str">
+        <f t="shared" si="49"/>
+        <v>font-size: clamp(1.2rem, 0.27vw + 1.12rem, 1.44rem);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.93</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="30"/>
+        <v>1.0356000000000001</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="31"/>
+        <v>1.0708</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="32"/>
+        <v>1.1178250000000001</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="33"/>
+        <v>1.194</v>
+      </c>
+      <c r="J18" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="44"/>
+        <v>16</v>
+      </c>
+      <c r="M18" s="7">
+        <f t="shared" si="45"/>
+        <v>16.569600000000001</v>
+      </c>
+      <c r="N18" s="7">
+        <f t="shared" si="46"/>
+        <v>17.1328</v>
+      </c>
+      <c r="O18" s="7">
+        <f t="shared" si="47"/>
+        <v>17.885200000000001</v>
+      </c>
+      <c r="P18" s="7">
+        <f t="shared" si="48"/>
+        <v>19.103999999999999</v>
+      </c>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="12" t="str">
+        <f t="shared" si="49"/>
+        <v>font-size: clamp(1rem, 0.22vw + 0.93rem, 1.2rem);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.83</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" ref="E19:E20" si="50">IF(($E$1/100*B19/16)+C19&lt;D19,D19,IF(($E$1/100*B19/16)+C19&gt;J19,J19,($E$1/100*B19/16)+C19))</f>
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" ref="F19:F20" si="51">IF(($F$1/100*B19/16)+C19&lt;D19,D19,IF(($F$1/100*B19/16)+C19&gt;J19,J19,($F$1/100*B19/16)+C19))</f>
+        <v>0.87119999999999997</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" ref="G19:G20" si="52">IF(($G$1/100*B19/16)+C19&lt;D19,D19,IF(($G$1/100*B19/16)+C19&gt;J19,J19,($G$1/100*B19/16)+C19))</f>
+        <v>0.90160000000000007</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" ref="H19:H20" si="53">IF(($H$1/100*B19/16)+C19&lt;D19,D19,IF(($H$1/100*B19/16)+C19&gt;J19,J19,($H$1/100*B19/16)+C19))</f>
+        <v>0.94221250000000001</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" ref="I19:I20" si="54">IF(($I$1/100*B19/16)+C19&lt;D19,D19,IF(($I$1/100*B19/16)+C19&gt;J19,J19,($I$1/100*B19/16)+C19))</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="9">
+        <v>1</v>
+      </c>
+      <c r="K19" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="L19" s="7">
+        <f t="shared" si="44"/>
+        <v>13.391999999999999</v>
+      </c>
+      <c r="M19" s="7">
+        <f t="shared" si="45"/>
+        <v>13.9392</v>
+      </c>
+      <c r="N19" s="7">
+        <f t="shared" si="46"/>
+        <v>14.425600000000001</v>
+      </c>
+      <c r="O19" s="7">
+        <f t="shared" si="47"/>
+        <v>15.0754</v>
+      </c>
+      <c r="P19" s="7">
+        <f t="shared" si="48"/>
+        <v>16</v>
+      </c>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="12" t="str">
+        <f t="shared" si="49"/>
+        <v>font-size: clamp(0.83rem, 0.19vw + 0.78rem, 1rem);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.69</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="50"/>
+        <v>0.69500000000000006</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="51"/>
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="52"/>
+        <v>0.746</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="53"/>
+        <v>0.77806249999999999</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="54"/>
+        <v>0.83000000000000007</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.83</v>
+      </c>
+      <c r="K20" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="L20" s="7">
+        <f t="shared" si="44"/>
+        <v>11.120000000000001</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" si="45"/>
+        <v>11.552</v>
+      </c>
+      <c r="N20" s="7">
+        <f t="shared" si="46"/>
+        <v>11.936</v>
+      </c>
+      <c r="O20" s="7">
+        <f t="shared" si="47"/>
+        <v>12.449</v>
+      </c>
+      <c r="P20" s="7">
+        <f t="shared" si="48"/>
+        <v>13.280000000000001</v>
+      </c>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="12" t="str">
+        <f t="shared" si="49"/>
+        <v>font-size: clamp(0.69rem, 0.15vw + 0.65rem, 0.83rem);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Updated the sizing spreadsheet.
</commit_message>
<xml_diff>
--- a/css_variable_font_sizes.xlsx
+++ b/css_variable_font_sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\code\css_modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\css_modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE73C59-9B3D-436D-8D46-4FA3B389656E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB682317-BDF3-468B-B37E-9073F3BADD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F820B3DE-D05A-4853-9D82-A8DA71430E49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F820B3DE-D05A-4853-9D82-A8DA71430E49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Heading</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>--step--2</t>
+  </si>
+  <si>
+    <t>padding</t>
+  </si>
+  <si>
+    <t>width</t>
   </si>
 </sst>
 </file>
@@ -570,23 +576,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5A6C22-BA9E-45E6-91AE-D25F7D23ED5A}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.69921875" style="2"/>
-    <col min="2" max="17" width="8.69921875" style="3"/>
-    <col min="18" max="18" width="9.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.69921875" style="1"/>
+    <col min="1" max="1" width="8.75" style="2"/>
+    <col min="2" max="17" width="8.75" style="3"/>
+    <col min="18" max="18" width="9.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -645,7 +651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -716,7 +722,7 @@
         <v>font-size: clamp(2rem, 1.5vw + 1.25rem, 3rem);</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -788,7 +794,7 @@
         <v>font-size: clamp(1.6rem, 1.2vw + 1rem, 2.4rem);</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -860,7 +866,7 @@
         <v>font-size: clamp(1.4rem, 1vw + 0.9rem, 2.1rem);</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -932,7 +938,7 @@
         <v>font-size: clamp(1.2rem, 0.85vw + 0.8rem, 1.8rem);</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>font-size: clamp(1.1rem, 0.7vw + 0.7rem, 1.5rem);</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>font-size: clamp(1rem, 0.55vw + 0.55rem, 1.2rem);</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>font-size: clamp(0.8rem, 0.55vw + 0.5rem, 1.1rem);</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>font-size: clamp(1.35rem, 1.75vw + 1rem, 3rem);</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>font-size: clamp(0.9rem, 0.55vw + 0.55rem, 1.1rem);</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1340,7 +1346,7 @@
         <v>font-size: clamp(0.8rem, 0.55vw + 0.5rem, 1rem);</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -1354,23 +1360,23 @@
         <v>0.9</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" ref="E12:E20" si="29">IF(($E$1/100*B12/16)+C12&lt;D12,D12,IF(($E$1/100*B12/16)+C12&gt;J12,J12,($E$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="E12:E18" si="29">IF(($E$1/100*B12/16)+C12&lt;D12,D12,IF(($E$1/100*B12/16)+C12&gt;J12,J12,($E$1/100*B12/16)+C12))</f>
         <v>0.9</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" ref="F12:F20" si="30">IF(($F$1/100*B12/16)+C12&lt;D12,D12,IF(($F$1/100*B12/16)+C12&gt;J12,J12,($F$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="F12:F18" si="30">IF(($F$1/100*B12/16)+C12&lt;D12,D12,IF(($F$1/100*B12/16)+C12&gt;J12,J12,($F$1/100*B12/16)+C12))</f>
         <v>0.9</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" ref="G12:G20" si="31">IF(($G$1/100*B12/16)+C12&lt;D12,D12,IF(($G$1/100*B12/16)+C12&gt;J12,J12,($G$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="G12:G18" si="31">IF(($G$1/100*B12/16)+C12&lt;D12,D12,IF(($G$1/100*B12/16)+C12&gt;J12,J12,($G$1/100*B12/16)+C12))</f>
         <v>0.95199999999999996</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" ref="H12:H19" si="32">IF(($H$1/100*B12/16)+C12&lt;D12,D12,IF(($H$1/100*B12/16)+C12&gt;J12,J12,($H$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="H12:H18" si="32">IF(($H$1/100*B12/16)+C12&lt;D12,D12,IF(($H$1/100*B12/16)+C12&gt;J12,J12,($H$1/100*B12/16)+C12))</f>
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" ref="I12:I19" si="33">IF(($I$1/100*B12/16)+C12&lt;D12,D12,IF(($I$1/100*B12/16)+C12&gt;J12,J12,($I$1/100*B12/16)+C12))</f>
+        <f t="shared" ref="I12:I18" si="33">IF(($I$1/100*B12/16)+C12&lt;D12,D12,IF(($I$1/100*B12/16)+C12&gt;J12,J12,($I$1/100*B12/16)+C12))</f>
         <v>1</v>
       </c>
       <c r="J12" s="9">
@@ -1380,23 +1386,23 @@
         <v>1</v>
       </c>
       <c r="L12" s="7">
-        <f t="shared" ref="L12:L18" si="34">E12*16</f>
+        <f t="shared" ref="L12" si="34">E12*16</f>
         <v>14.4</v>
       </c>
       <c r="M12" s="7">
-        <f t="shared" ref="M12:M18" si="35">F12*16</f>
+        <f t="shared" ref="M12" si="35">F12*16</f>
         <v>14.4</v>
       </c>
       <c r="N12" s="7">
-        <f t="shared" ref="N12:N18" si="36">G12*16</f>
+        <f t="shared" ref="N12" si="36">G12*16</f>
         <v>15.231999999999999</v>
       </c>
       <c r="O12" s="7">
-        <f t="shared" ref="O12:O18" si="37">H12*16</f>
+        <f t="shared" ref="O12" si="37">H12*16</f>
         <v>16</v>
       </c>
       <c r="P12" s="7">
-        <f t="shared" ref="P12:P18" si="38">I12*16</f>
+        <f t="shared" ref="P12" si="38">I12*16</f>
         <v>16</v>
       </c>
       <c r="Q12" s="14"/>
@@ -1406,7 +1412,7 @@
         <v>font-size: clamp(0.9rem, 0.55vw + 0.6rem, 1rem);</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1468,11 +1474,11 @@
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
       <c r="S13" s="12" t="str">
-        <f t="shared" ref="S13:S20" si="49">"font-size: clamp("&amp;D13&amp;"rem, "&amp;B13&amp;"vw + "&amp;C13&amp;"rem, "&amp;J13&amp;"rem);"</f>
+        <f t="shared" ref="S13:S21" si="49">"font-size: clamp("&amp;D13&amp;"rem, "&amp;B13&amp;"vw + "&amp;C13&amp;"rem, "&amp;J13&amp;"rem);"</f>
         <v>font-size: clamp(2.49rem, 0.55vw + 2.32rem, 2.99rem);</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>font-size: clamp(2.07rem, 0.46vw + 1.94rem, 2.49rem);</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1604,7 +1610,7 @@
         <v>font-size: clamp(1.73rem, 0.38vw + 1.61rem, 2.07rem);</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
@@ -1670,7 +1676,7 @@
         <v>font-size: clamp(1.44rem, 0.32vw + 1.34rem, 1.73rem);</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1736,7 +1742,7 @@
         <v>font-size: clamp(1.2rem, 0.27vw + 1.12rem, 1.44rem);</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>font-size: clamp(1rem, 0.22vw + 0.93rem, 1.2rem);</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>26</v>
       </c>
@@ -1868,7 +1874,7 @@
         <v>font-size: clamp(0.83rem, 0.19vw + 0.78rem, 1rem);</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>27</v>
       </c>
@@ -1934,26 +1940,221 @@
         <v>font-size: clamp(0.69rem, 0.15vw + 0.65rem, 0.83rem);</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+    <row r="21" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" ref="E21:E22" si="55">IF(($E$1/100*B21/16)+C21&lt;D21,D21,IF(($E$1/100*B21/16)+C21&gt;J21,J21,($E$1/100*B21/16)+C21))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" ref="F21:F22" si="56">IF(($F$1/100*B21/16)+C21&lt;D21,D21,IF(($F$1/100*B21/16)+C21&gt;J21,J21,($F$1/100*B21/16)+C21))</f>
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" ref="G21:G22" si="57">IF(($G$1/100*B21/16)+C21&lt;D21,D21,IF(($G$1/100*B21/16)+C21&gt;J21,J21,($G$1/100*B21/16)+C21))</f>
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" ref="H21:H22" si="58">IF(($H$1/100*B21/16)+C21&lt;D21,D21,IF(($H$1/100*B21/16)+C21&gt;J21,J21,($H$1/100*B21/16)+C21))</f>
+        <v>0.57806250000000003</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" ref="I21:I22" si="59">IF(($I$1/100*B21/16)+C21&lt;D21,D21,IF(($I$1/100*B21/16)+C21&gt;J21,J21,($I$1/100*B21/16)+C21))</f>
+        <v>0.63</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.63</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="L21" s="7">
+        <f t="shared" ref="L21:L22" si="60">E21*16</f>
+        <v>8</v>
+      </c>
+      <c r="M21" s="7">
+        <f t="shared" ref="M21:M22" si="61">F21*16</f>
+        <v>8.3520000000000003</v>
+      </c>
+      <c r="N21" s="7">
+        <f t="shared" ref="N21:N22" si="62">G21*16</f>
+        <v>8.7360000000000007</v>
+      </c>
+      <c r="O21" s="7">
+        <f t="shared" ref="O21:O22" si="63">H21*16</f>
+        <v>9.2490000000000006</v>
+      </c>
+      <c r="P21" s="7">
+        <f t="shared" ref="P21:P22" si="64">I21*16</f>
+        <v>10.08</v>
+      </c>
       <c r="Q21" s="14"/>
       <c r="R21" s="14"/>
-      <c r="S21" s="12"/>
+      <c r="S21" s="12" t="str">
+        <f>"font-size: clamp("&amp;D21&amp;"rem, "&amp;B21&amp;"vw + "&amp;C21&amp;"rem, "&amp;J21&amp;"rem);"</f>
+        <v>font-size: clamp(0.5rem, 0.15vw + 0.45rem, 0.63rem);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2.67</v>
+      </c>
+      <c r="D22" s="9">
+        <v>3</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="55"/>
+        <v>3</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="56"/>
+        <v>3.198</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="57"/>
+        <v>3.3740000000000001</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="58"/>
+        <v>3.6091250000000001</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="59"/>
+        <v>3.99</v>
+      </c>
+      <c r="J22" s="9">
+        <v>4</v>
+      </c>
+      <c r="K22" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="L22" s="7">
+        <f t="shared" si="60"/>
+        <v>48</v>
+      </c>
+      <c r="M22" s="7">
+        <f t="shared" si="61"/>
+        <v>51.167999999999999</v>
+      </c>
+      <c r="N22" s="7">
+        <f t="shared" si="62"/>
+        <v>53.984000000000002</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" si="63"/>
+        <v>57.746000000000002</v>
+      </c>
+      <c r="P22" s="7">
+        <f t="shared" si="64"/>
+        <v>63.84</v>
+      </c>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="12" t="str">
+        <f>"font-size: clamp("&amp;D22&amp;"rem, "&amp;B22&amp;"vw + "&amp;C22&amp;"rem, "&amp;J22&amp;"rem);"</f>
+        <v>font-size: clamp(3rem, 1.1vw + 2.67rem, 4rem);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="12"/>
+    </row>
+    <row r="24" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="12"/>
+    </row>
+    <row r="25" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="12"/>
+    </row>
+    <row r="26" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>